<commit_message>
added the link names not matching defect on the rtm and defect report
</commit_message>
<xml_diff>
--- a/Bug-Catcher-Requirements-Traceability-Matrix-Template-Lei.xlsx
+++ b/Bug-Catcher-Requirements-Traceability-Matrix-Template-Lei.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frejusgnonsey/Documents/Revature/Lei_FoundationsProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD16C9C0-7BF8-EE45-BBC2-79F5EDF8042D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58197913-BCEF-C34B-86F8-1F1F14449586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="500" windowWidth="22480" windowHeight="13580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
   <si>
     <t>RequirementID</t>
   </si>
@@ -198,7 +198,10 @@
     <t>Defects can be successfully reported if steps given are too short, as defect text area does not have minimum characters input</t>
   </si>
   <si>
-    <t>Original steps could be replicated</t>
+    <t>Original steps could not be replicated</t>
+  </si>
+  <si>
+    <t>The page title was not matching the same given in the feature file</t>
   </si>
 </sst>
 </file>
@@ -715,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -874,7 +877,12 @@
       <c r="F7" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="10"/>
+      <c r="G7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="10">
+        <v>903</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13">

</xml_diff>